<commit_message>
endogenous BAF, fixed gene names
</commit_message>
<xml_diff>
--- a/cofactor_complexes/data/cofactor_complexes_manual.xlsx
+++ b/cofactor_complexes/data/cofactor_complexes_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinseylong/Desktop/StallerRotation/cofactor_complexes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8319E815-87BB-2F44-ADA7-5F590A76D133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D5F9A40-737F-C64E-B249-C91B6B90FC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16460" xr2:uid="{60EE9497-BA39-A349-9E49-7CEF518C88CE}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="P300-CBP" sheetId="5" r:id="rId4"/>
     <sheet name="SAGA" sheetId="6" r:id="rId5"/>
     <sheet name="TFIID" sheetId="4" r:id="rId6"/>
-    <sheet name="Others" sheetId="7" r:id="rId7"/>
+    <sheet name="other" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="331">
   <si>
     <t>Complex</t>
   </si>
@@ -437,9 +437,6 @@
     <t>H2AZ</t>
   </si>
   <si>
-    <t>H2B</t>
-  </si>
-  <si>
     <t>Yang et al. 2024</t>
   </si>
   <si>
@@ -650,9 +647,6 @@
     <t>Goodrich and Tijian, 2027</t>
   </si>
   <si>
-    <t>FT2B</t>
-  </si>
-  <si>
     <t>TFIIB</t>
   </si>
   <si>
@@ -701,15 +695,9 @@
     <t>CCNH</t>
   </si>
   <si>
-    <t>GTFH2</t>
-  </si>
-  <si>
     <t>MNAT1</t>
   </si>
   <si>
-    <t>GTFH2H4</t>
-  </si>
-  <si>
     <t>FACT</t>
   </si>
   <si>
@@ -797,9 +785,6 @@
     <t>RBBP5</t>
   </si>
   <si>
-    <t>MENIN</t>
-  </si>
-  <si>
     <t>KMT2A</t>
   </si>
   <si>
@@ -1007,9 +992,6 @@
     <t>[SMARCA4]</t>
   </si>
   <si>
-    <t>BCL7</t>
-  </si>
-  <si>
     <t>ACTL6A</t>
   </si>
   <si>
@@ -1032,6 +1014,27 @@
   </si>
   <si>
     <t>DPF2</t>
+  </si>
+  <si>
+    <t>GTF2H4</t>
+  </si>
+  <si>
+    <t>GTF2B</t>
+  </si>
+  <si>
+    <t>MEN1</t>
+  </si>
+  <si>
+    <t>GTF2H2</t>
+  </si>
+  <si>
+    <t>H2BC21</t>
+  </si>
+  <si>
+    <t>histone H2B</t>
+  </si>
+  <si>
+    <t>Mashtalir, Suzuki ,Farrell, Sankar, et al. Cell (2021)</t>
   </si>
 </sst>
 </file>
@@ -1409,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDCAA04-1F14-EA49-A1DF-5D501BCF1BAE}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="187" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,7 +1427,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2483,193 +2486,275 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>302</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" t="s">
+        <v>312</v>
+      </c>
+      <c r="D65" t="s">
+        <v>314</v>
+      </c>
+      <c r="G65" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>313</v>
+      </c>
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" t="s">
+        <v>312</v>
+      </c>
+      <c r="D66" t="s">
+        <v>315</v>
+      </c>
+      <c r="G66" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67" t="s">
+        <v>312</v>
+      </c>
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
+      <c r="G67" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" t="s">
+        <v>312</v>
+      </c>
+      <c r="D68" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69" t="s">
+        <v>312</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" t="s">
+        <v>312</v>
+      </c>
+      <c r="G70" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>316</v>
+      </c>
+      <c r="B71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" t="s">
+        <v>312</v>
+      </c>
+      <c r="G71" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>305</v>
+      </c>
+      <c r="B72" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72" t="s">
+        <v>312</v>
+      </c>
+      <c r="D72" t="s">
+        <v>317</v>
+      </c>
+      <c r="G72" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>306</v>
+      </c>
+      <c r="B73" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" t="s">
+        <v>312</v>
+      </c>
+      <c r="D73" t="s">
+        <v>318</v>
+      </c>
+      <c r="G73" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>309</v>
+      </c>
+      <c r="B74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" t="s">
+        <v>312</v>
+      </c>
+      <c r="G74" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>303</v>
+      </c>
+      <c r="B75" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" t="s">
+        <v>312</v>
+      </c>
+      <c r="D75" t="s">
+        <v>319</v>
+      </c>
+      <c r="G75" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>307</v>
       </c>
-      <c r="B65" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" t="s">
-        <v>317</v>
-      </c>
-      <c r="D65" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>318</v>
-      </c>
-      <c r="B66" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" t="s">
-        <v>317</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="B76" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" t="s">
+        <v>312</v>
+      </c>
+      <c r="D76" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="G76" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" t="s">
+        <v>312</v>
+      </c>
+      <c r="G77" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78" t="s">
+        <v>312</v>
+      </c>
+      <c r="D78" t="s">
         <v>321</v>
       </c>
-      <c r="B67" t="s">
-        <v>61</v>
-      </c>
-      <c r="C67" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" t="s">
-        <v>61</v>
-      </c>
-      <c r="C68" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="G78" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>296</v>
+      </c>
+      <c r="B79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>312</v>
+      </c>
+      <c r="D79" t="s">
         <v>322</v>
       </c>
-      <c r="B69" t="s">
-        <v>61</v>
-      </c>
-      <c r="C69" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>310</v>
-      </c>
-      <c r="B70" t="s">
-        <v>61</v>
-      </c>
-      <c r="C70" t="s">
-        <v>317</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="G79" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>311</v>
-      </c>
-      <c r="B71" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" t="s">
-        <v>317</v>
-      </c>
-      <c r="D71" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>314</v>
-      </c>
-      <c r="B72" t="s">
-        <v>61</v>
-      </c>
-      <c r="C72" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>308</v>
-      </c>
-      <c r="B73" t="s">
-        <v>61</v>
-      </c>
-      <c r="C73" t="s">
-        <v>317</v>
-      </c>
-      <c r="D73" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B80" t="s">
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
         <v>312</v>
       </c>
-      <c r="B74" t="s">
-        <v>61</v>
-      </c>
-      <c r="C74" t="s">
-        <v>317</v>
-      </c>
-      <c r="D74" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="G80" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>300</v>
       </c>
-      <c r="B76" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" t="s">
-        <v>317</v>
-      </c>
-      <c r="D76" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>301</v>
-      </c>
-      <c r="B77" t="s">
-        <v>61</v>
-      </c>
-      <c r="C77" t="s">
-        <v>317</v>
-      </c>
-      <c r="D77" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>329</v>
-      </c>
-      <c r="B78" t="s">
-        <v>61</v>
-      </c>
-      <c r="C78" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>305</v>
-      </c>
-      <c r="B79" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" t="s">
-        <v>317</v>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C81" t="s">
+        <v>312</v>
+      </c>
+      <c r="G81" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2695,7 +2780,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3219,14 +3304,14 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3258,7 +3343,7 @@
         <v>121</v>
       </c>
       <c r="G2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3272,7 +3357,7 @@
         <v>119</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -3286,7 +3371,7 @@
         <v>122</v>
       </c>
       <c r="G4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3300,7 +3385,7 @@
         <v>122</v>
       </c>
       <c r="G5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -3314,7 +3399,7 @@
         <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3328,7 +3413,7 @@
         <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -3342,7 +3427,7 @@
         <v>126</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3356,7 +3441,7 @@
         <v>126</v>
       </c>
       <c r="G9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3370,7 +3455,7 @@
         <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3384,7 +3469,7 @@
         <v>126</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3398,12 +3483,12 @@
         <v>126</v>
       </c>
       <c r="G12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>328</v>
       </c>
       <c r="B13" t="s">
         <v>120</v>
@@ -3411,8 +3496,11 @@
       <c r="C13" t="s">
         <v>126</v>
       </c>
+      <c r="F13" t="s">
+        <v>329</v>
+      </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3433,7 +3521,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3456,24 +3544,24 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
         <v>133</v>
-      </c>
-      <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
         <v>135</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3485,15 +3573,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B8B951-EA8E-2E4C-BA7C-5C07EA606FEE}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="200" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3516,268 +3604,268 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
         <v>144</v>
       </c>
-      <c r="C2" t="s">
-        <v>145</v>
-      </c>
       <c r="G2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>144</v>
       </c>
-      <c r="C3" t="s">
-        <v>145</v>
-      </c>
       <c r="G3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" t="s">
-        <v>145</v>
-      </c>
       <c r="G4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
         <v>144</v>
       </c>
-      <c r="C5" t="s">
-        <v>145</v>
-      </c>
       <c r="G5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
         <v>115</v>
       </c>
       <c r="G6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
         <v>115</v>
       </c>
       <c r="G7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
         <v>115</v>
       </c>
       <c r="G8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
       </c>
       <c r="G9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" t="s">
-        <v>154</v>
-      </c>
       <c r="G10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" t="s">
         <v>164</v>
       </c>
-      <c r="B20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C20" t="s">
-        <v>165</v>
-      </c>
       <c r="G20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3785,13 +3873,13 @@
         <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
         <v>117</v>
       </c>
       <c r="G21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3804,15 +3892,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBC8008-1482-DD4C-8534-3B9EA20AED77}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="186" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="186" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3835,254 +3923,254 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
         <v>169</v>
       </c>
-      <c r="B3" t="s">
-        <v>170</v>
-      </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4095,15 +4183,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6D59F6-3161-E64B-986F-0BB1F15100DC}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="171" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:B78"/>
+    <sheetView zoomScale="171" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4126,482 +4214,482 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>327</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>324</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B21" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B23" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B25" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B26" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B28" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B30" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B31" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B32" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B33" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B35" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B36" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B37" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B39" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B40" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B41" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>251</v>
+        <v>326</v>
       </c>
       <c r="B42" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B43" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B44" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B45" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B46" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B47" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B48" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B49" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B50" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B51" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B52" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B54" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B55" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B56" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B57" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B58" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B61" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -4609,279 +4697,279 @@
         <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B63" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B64" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B69" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B70" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B71" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B72" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B73" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B74" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B75" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B76" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B77" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B78" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B79" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B80" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B81" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B82" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B83" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B84" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B85" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B86" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B87" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B88" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B89" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B90" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B91" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B92" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B93" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B94" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B95" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B96" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -4889,7 +4977,7 @@
         <v>128</v>
       </c>
       <c r="B97" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -4897,87 +4985,87 @@
         <v>129</v>
       </c>
       <c r="B98" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B99" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B100" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B101" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B102" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B103" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B104" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B105" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B106" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B107" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B108" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -4985,15 +5073,15 @@
         <v>7</v>
       </c>
       <c r="B109" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B110" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>